<commit_message>
Continued revisions for Table S1.
</commit_message>
<xml_diff>
--- a/Table2_flexible.xlsx
+++ b/Table2_flexible.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennarewcastle/Desktop/Desktop/Research Files/Bog Project/New Bog Stuff/Bog2015_R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{86EA0E92-075A-9D44-9A25-AA48C1523104}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673C3F8D-0EE1-9F40-AB47-45D9A8D96732}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="980" windowWidth="27640" windowHeight="16040"/>
+    <workbookView xWindow="1160" yWindow="8880" windowWidth="27640" windowHeight="9160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table2" sheetId="1" r:id="rId1"/>
+    <sheet name="Table1" sheetId="2" r:id="rId1"/>
+    <sheet name="Table2" sheetId="1" r:id="rId2"/>
+    <sheet name="Table S1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Response</t>
   </si>
@@ -117,12 +119,51 @@
       <t>2</t>
     </r>
   </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Heterotrophic Respiration</t>
+  </si>
+  <si>
+    <t>Microbial Biomass Carbon (MBC)</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>Dissolved Organic Carbon (DOC)</t>
+  </si>
+  <si>
+    <t>Peat C:N</t>
+  </si>
+  <si>
+    <t>BG Enzyme Activity</t>
+  </si>
+  <si>
+    <t>AG Enzyme Activity</t>
+  </si>
+  <si>
+    <t>CBH Enzyme Activity</t>
+  </si>
+  <si>
+    <t>NAG Enzyme Activity</t>
+  </si>
+  <si>
+    <t>LAP Enzyme Activity</t>
+  </si>
+  <si>
+    <t>PHOS Enzyme Activity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -293,8 +334,29 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,8 +542,14 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -616,6 +684,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -661,7 +740,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,6 +779,30 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1055,10 +1158,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F85BCFB-4843-3348-85C7-7A7563AFB74D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
@@ -1193,4 +1308,166 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8F2ACB-8872-BB44-B8B9-3510863E722F}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20" thickBot="1">
+      <c r="A1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="18">
+        <v>-0.63</v>
+      </c>
+      <c r="C2" s="18">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="20">
+        <v>-0.98</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.43</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="20">
+        <v>-1.37</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="18">
+        <v>-1.42</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="20">
+        <v>0.91</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="18">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="20">
+        <v>-1.42</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="18">
+        <v>-0.16</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="C11" s="20">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="18">
+        <v>-0.11</v>
+      </c>
+      <c r="C12" s="18">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" thickBot="1">
+      <c r="A13" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="22">
+        <v>-1.27</v>
+      </c>
+      <c r="C13" s="22">
+        <v>0.21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>